<commit_message>
Filters schedule and adds courses as needed - working
</commit_message>
<xml_diff>
--- a/course_rotations.xlsx
+++ b/course_rotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\57100_AI_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E188F7-1BC2-4A00-A417-94FC2403F7D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8C6B18-C6E6-468D-8C9A-1B51E31667F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{1CD8CD11-57A3-4341-BDA0-459356E630BB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12195" xr2:uid="{1CD8CD11-57A3-4341-BDA0-459356E630BB}"/>
   </bookViews>
   <sheets>
     <sheet name="course_rotations" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="35">
   <si>
     <t>course_name</t>
   </si>
@@ -490,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C61E35-95D2-D642-9024-291B5BDC3312}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -576,27 +576,27 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+    <row r="3" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>33</v>
@@ -613,86 +613,86 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
+        <v>28</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" t="s">
-        <v>33</v>
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>29</v>
@@ -718,16 +718,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>29</v>
@@ -753,16 +753,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>29</v>
@@ -788,16 +788,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>29</v>
@@ -823,16 +823,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>29</v>
@@ -858,19 +858,19 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
@@ -893,19 +893,19 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
         <v>33</v>
@@ -928,16 +928,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>30</v>
@@ -963,16 +963,16 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>30</v>
@@ -998,16 +998,16 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>30</v>
@@ -1033,10 +1033,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -1068,71 +1068,141 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>3</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" t="s">
-        <v>33</v>
-      </c>
-      <c r="K17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="2">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B20" s="2">
+        <v>4</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K18" s="2" t="s">
+      <c r="F20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Program working - need to expand constraints and course schedule
</commit_message>
<xml_diff>
--- a/course_rotations.xlsx
+++ b/course_rotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\57100_AI_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8C6B18-C6E6-468D-8C9A-1B51E31667F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DB8241-D4DF-4EEA-84DC-5317DE64BC48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12195" xr2:uid="{1CD8CD11-57A3-4341-BDA0-459356E630BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="44">
   <si>
     <t>course_name</t>
   </si>
@@ -65,69 +65,15 @@
     <t>tuesday</t>
   </si>
   <si>
-    <t>CPSC-50100</t>
-  </si>
-  <si>
-    <t>MATH-51000</t>
-  </si>
-  <si>
-    <t>MATH-51100</t>
-  </si>
-  <si>
-    <t>MATH-51200</t>
-  </si>
-  <si>
-    <t>CPSC-51000</t>
-  </si>
-  <si>
-    <t>CPSC-51100</t>
-  </si>
-  <si>
-    <t>CPSC-53000</t>
-  </si>
-  <si>
-    <t>CPSC-54000</t>
-  </si>
-  <si>
-    <t>CPSC-55000</t>
-  </si>
-  <si>
-    <t>CPSC-50600</t>
-  </si>
-  <si>
-    <t>CPSC-51700</t>
-  </si>
-  <si>
-    <t>CPSC-52500</t>
-  </si>
-  <si>
-    <t>CPSC-55200</t>
-  </si>
-  <si>
-    <t>CPSC-55500</t>
-  </si>
-  <si>
-    <t>CPSC-57400</t>
-  </si>
-  <si>
-    <t>CPSC-59000</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
-    <t>foundation</t>
-  </si>
-  <si>
     <t>core</t>
   </si>
   <si>
     <t>elective</t>
   </si>
   <si>
-    <t>capstone</t>
-  </si>
-  <si>
     <t>evening</t>
   </si>
   <si>
@@ -135,6 +81,87 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Course A</t>
+  </si>
+  <si>
+    <t>Course B</t>
+  </si>
+  <si>
+    <t>Course C</t>
+  </si>
+  <si>
+    <t>Course D</t>
+  </si>
+  <si>
+    <t>Course E</t>
+  </si>
+  <si>
+    <t>Course F</t>
+  </si>
+  <si>
+    <t>Course G</t>
+  </si>
+  <si>
+    <t>Course H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course I </t>
+  </si>
+  <si>
+    <t>Course J</t>
+  </si>
+  <si>
+    <t>Course L</t>
+  </si>
+  <si>
+    <t>Course K</t>
+  </si>
+  <si>
+    <t>Course M</t>
+  </si>
+  <si>
+    <t>Course N</t>
+  </si>
+  <si>
+    <t>Course O</t>
+  </si>
+  <si>
+    <t>Course P</t>
+  </si>
+  <si>
+    <t>Course Q</t>
+  </si>
+  <si>
+    <t>Course R</t>
+  </si>
+  <si>
+    <t>Course S</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>Course T</t>
+  </si>
+  <si>
+    <t>Course U</t>
+  </si>
+  <si>
+    <t>Course V</t>
+  </si>
+  <si>
+    <t>Course W</t>
+  </si>
+  <si>
+    <t>Course X</t>
+  </si>
+  <si>
+    <t>Course Z</t>
+  </si>
+  <si>
+    <t>final</t>
   </si>
 </sst>
 </file>
@@ -490,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C61E35-95D2-D642-9024-291B5BDC3312}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -502,11 +529,11 @@
     <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.875" customWidth="1"/>
-    <col min="12" max="13" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +547,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F1">
         <v>1</v>
@@ -531,19 +558,10 @@
       <c r="H1">
         <v>3</v>
       </c>
-      <c r="I1">
-        <v>4</v>
-      </c>
-      <c r="J1">
-        <v>5</v>
-      </c>
-      <c r="K1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -555,30 +573,21 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -590,65 +599,47 @@
         <v>6</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
@@ -660,65 +651,47 @@
         <v>10</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -730,30 +703,21 @@
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -765,30 +729,21 @@
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -800,30 +755,21 @@
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -835,30 +781,21 @@
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -870,30 +807,21 @@
         <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -905,30 +833,21 @@
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -939,31 +858,22 @@
       <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
+      <c r="E13" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -974,31 +884,22 @@
       <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1010,30 +911,21 @@
         <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -1045,30 +937,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16" t="s">
-        <v>33</v>
-      </c>
-      <c r="J16" t="s">
-        <v>33</v>
-      </c>
-      <c r="K16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -1080,30 +963,21 @@
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="G17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" t="s">
-        <v>33</v>
-      </c>
-      <c r="K17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1115,95 +989,250 @@
         <v>6</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="4">
+        <v>5</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="4">
         <v>3</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="4">
+        <v>4</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="4">
+        <v>2</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" t="s">
-        <v>33</v>
-      </c>
-      <c r="J19" t="s">
-        <v>33</v>
-      </c>
-      <c r="K19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="2">
-        <v>4</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="E25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="2">
+        <v>4</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>33</v>
+      <c r="E26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Works for 3 courses per semester
</commit_message>
<xml_diff>
--- a/course_rotations.xlsx
+++ b/course_rotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\57100_AI_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DB8241-D4DF-4EEA-84DC-5317DE64BC48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35A5154-444B-457E-9B44-606EA0DA62BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12195" xr2:uid="{1CD8CD11-57A3-4341-BDA0-459356E630BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="44">
   <si>
     <t>course_name</t>
   </si>
@@ -517,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C61E35-95D2-D642-9024-291B5BDC3312}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,7 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -587,16 +587,16 @@
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>36</v>
@@ -605,33 +605,33 @@
         <v>15</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>16</v>
@@ -639,33 +639,33 @@
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -674,82 +674,82 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
+        <v>36</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4">
+        <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>15</v>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -769,16 +769,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>12</v>
@@ -795,16 +795,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>12</v>
@@ -821,16 +821,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>12</v>
@@ -847,18 +847,18 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F13" t="s">
@@ -873,18 +873,18 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" t="s">
@@ -899,19 +899,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
         <v>15</v>
@@ -925,18 +925,18 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F16" t="s">
@@ -951,18 +951,18 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F17" t="s">
@@ -977,16 +977,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>13</v>
@@ -1001,96 +1001,96 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="4">
-        <v>2</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="4" t="s">
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B22" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>13</v>
@@ -1107,16 +1107,16 @@
     </row>
     <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B23" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>13</v>
@@ -1133,16 +1133,16 @@
     </row>
     <row r="24" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B24" s="4">
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>13</v>
@@ -1157,85 +1157,164 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25">
+    <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="4">
         <v>3</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="D25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="2">
+      <c r="F25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="4">
         <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="4">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="F29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>42</v>
       </c>
-      <c r="B27">
+      <c r="B30">
         <v>3</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>14</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D30" t="s">
         <v>6</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E30" t="s">
         <v>43</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F30" t="s">
         <v>16</v>
       </c>
-      <c r="G27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Electives will now be added that have the highest professor rating
</commit_message>
<xml_diff>
--- a/course_rotations.xlsx
+++ b/course_rotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\57100_AI_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35A5154-444B-457E-9B44-606EA0DA62BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA0BF3A-19D8-4452-A7D2-90728BE633E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12195" xr2:uid="{1CD8CD11-57A3-4341-BDA0-459356E630BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="44">
   <si>
     <t>course_name</t>
   </si>
@@ -517,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C61E35-95D2-D642-9024-291B5BDC3312}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -741,44 +741,44 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9">
-        <v>3</v>
+      <c r="B9" s="4">
+        <v>4</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="F9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>12</v>
@@ -790,18 +790,18 @@
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -813,50 +813,50 @@
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
+    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="F12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>12</v>
@@ -873,16 +873,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
@@ -897,47 +897,47 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="F15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
@@ -951,19 +951,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -977,19 +977,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
         <v>15</v>
@@ -1003,18 +1003,18 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F19" t="s">
@@ -1029,18 +1029,18 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F20" t="s">
@@ -1055,16 +1055,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>13</v>
@@ -1079,96 +1079,96 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="4">
-        <v>5</v>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="4">
-        <v>1</v>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="4">
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="4" t="s">
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B25" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>13</v>
@@ -1185,16 +1185,16 @@
     </row>
     <row r="26" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B26" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>13</v>
@@ -1211,16 +1211,16 @@
     </row>
     <row r="27" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B27" s="4">
         <v>2</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>13</v>
@@ -1235,81 +1235,159 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="4">
+        <v>3</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="4">
+        <v>4</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="4">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B28">
+      <c r="B31">
         <v>3</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="2">
-        <v>4</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="B32" s="2">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="F32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>42</v>
       </c>
-      <c r="B30">
+      <c r="B33">
         <v>3</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C33" t="s">
         <v>14</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D33" t="s">
         <v>6</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E33" t="s">
         <v>43</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F33" t="s">
         <v>16</v>
       </c>
-      <c r="G30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>